<commit_message>
Added IECMaterials download template
</commit_message>
<xml_diff>
--- a/src/templates/IECMaterials_Template.xlsx
+++ b/src/templates/IECMaterials_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devvi\Documents\GitHub\TAD-Reports-BE\src\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C57E14-B7CE-4B87-B47C-FCB190B98E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD3D960-D0D9-4534-96E3-65365AF85BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>Barangay</t>
   </si>
   <si>
-    <t>Remarks</t>
-  </si>
-  <si>
     <t>District</t>
   </si>
   <si>
@@ -66,18 +63,6 @@
     <t>Regional Office 4</t>
   </si>
   <si>
-    <t>Oriental Mindoro</t>
-  </si>
-  <si>
-    <t>Calapan</t>
-  </si>
-  <si>
-    <t>Caaguyuan</t>
-  </si>
-  <si>
-    <t>Training Upload Form</t>
-  </si>
-  <si>
     <t>District 1</t>
   </si>
   <si>
@@ -90,16 +75,31 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Conduct of Training</t>
-  </si>
-  <si>
-    <t>Venue</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
+    <t>Title of IEC Material</t>
+  </si>
+  <si>
+    <t>No of Copies Distributed</t>
+  </si>
+  <si>
+    <t>Date Distributed</t>
+  </si>
+  <si>
+    <t>IEC Materials Upload Form</t>
+  </si>
+  <si>
+    <t>Youth</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Magdalo</t>
+  </si>
+  <si>
+    <t>San Fabian</t>
+  </si>
+  <si>
+    <t>Pangasinan</t>
   </si>
 </sst>
 </file>
@@ -245,18 +245,18 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="12" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="12" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="12" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="12" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="12" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="12" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -264,12 +264,12 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="12" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="12" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -497,83 +497,75 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15" style="2" customWidth="1"/>
-    <col min="3" max="6" width="20" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="34.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15" style="2" customWidth="1"/>
-    <col min="10" max="10" width="20" style="2" customWidth="1"/>
-    <col min="11" max="12" width="20.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="30" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="12.5703125" style="2"/>
+    <col min="1" max="3" width="15" style="2" customWidth="1"/>
+    <col min="4" max="7" width="20" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="34.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="10"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="10"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="10"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="10"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -581,51 +573,43 @@
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="7" t="s">
+    </row>
+    <row r="5" spans="1:11" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="I5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -635,49 +619,45 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="4"/>
+      <c r="J6" s="3"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+    </row>
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>44553</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8">
+        <v>500</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="G7" s="5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="5">
-        <v>10000</v>
-      </c>
-      <c r="J7" s="6">
-        <v>300</v>
-      </c>
-      <c r="K7" s="6">
-        <v>300</v>
-      </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="11">
-        <v>44553</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="12">
+        <v>44938</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -687,12 +667,10 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="4"/>
+      <c r="J8" s="3"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -702,12 +680,10 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="4"/>
+      <c r="J9" s="3"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -717,12 +693,10 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="4"/>
+      <c r="J10" s="3"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -732,12 +706,10 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="4"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -747,12 +719,10 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="3"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -762,12 +732,10 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="4"/>
+      <c r="J13" s="3"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -777,12 +745,10 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="4"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -792,12 +758,10 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="4"/>
+      <c r="J15" s="3"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -807,12 +771,10 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="4"/>
+      <c r="J16" s="3"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="3"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -822,12 +784,10 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="4"/>
+      <c r="J17" s="3"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -837,12 +797,10 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="4"/>
+      <c r="J18" s="3"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -852,12 +810,10 @@
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="4"/>
+      <c r="J19" s="3"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -869,10 +825,8 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -884,10 +838,8 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -899,10 +851,8 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -914,10 +864,8 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -929,10 +877,8 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -944,10 +890,8 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -959,10 +903,8 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -974,10 +916,8 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -989,10 +929,8 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1004,10 +942,8 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1019,10 +955,8 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1034,10 +968,8 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1049,10 +981,8 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-    </row>
-    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1064,10 +994,8 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-    </row>
-    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1079,10 +1007,8 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-    </row>
-    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1094,10 +1020,8 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-    </row>
-    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1109,10 +1033,8 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-    </row>
-    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1124,10 +1046,8 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1139,10 +1059,8 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1154,10 +1072,8 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-    </row>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1169,10 +1085,8 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-    </row>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1184,10 +1098,8 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-    </row>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1199,10 +1111,8 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-    </row>
-    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1214,16 +1124,14 @@
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="D4:K4"/>
-    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="E4:K4"/>
+    <mergeCell ref="E3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>